<commit_message>
fixing more vbc data
</commit_message>
<xml_diff>
--- a/data/imports/envisio-import-safety.xlsx
+++ b/data/imports/envisio-import-safety.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Phoenix</t>
   </si>
@@ -971,10 +971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,7 +986,7 @@
     <col min="7" max="7" width="18.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -994,38 +994,66 @@
         <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>61</v>
+      <c r="C2" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1033,20 +1061,34 @@
         <v>100000</v>
       </c>
       <c r="C3" s="4">
-        <v>3.5</v>
+        <v>221</v>
       </c>
       <c r="D3" s="4">
-        <v>38.799999999999997</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4">
-        <v>0.38</v>
+        <v>57.16</v>
       </c>
       <c r="F3" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44.29</v>
+      </c>
+      <c r="G3" s="4">
+        <v>22.18</v>
+      </c>
+      <c r="H3" s="4">
+        <v>31.61</v>
+      </c>
+      <c r="I3" s="4">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="K3" s="4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1054,20 +1096,34 @@
         <v>100001</v>
       </c>
       <c r="C4" s="4">
-        <v>1.9</v>
+        <v>498</v>
       </c>
       <c r="D4" s="4">
-        <v>23.3</v>
+        <v>5.2</v>
       </c>
       <c r="E4" s="4">
-        <v>0.39</v>
+        <v>43.47</v>
       </c>
       <c r="F4" s="4">
-        <v>0.18</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26.35</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24.51</v>
+      </c>
+      <c r="H4" s="4">
+        <v>26.35</v>
+      </c>
+      <c r="I4" s="4">
+        <v>15.97</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="K4" s="4">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1075,20 +1131,34 @@
         <v>100002</v>
       </c>
       <c r="C5" s="4">
-        <v>0.9</v>
+        <v>257</v>
       </c>
       <c r="D5" s="4">
-        <v>14.8</v>
+        <v>16.5</v>
       </c>
       <c r="E5" s="4">
-        <v>0.58599999999999997</v>
+        <v>40.67</v>
       </c>
       <c r="F5" s="4">
-        <v>0.249</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30.78</v>
+      </c>
+      <c r="G5" s="4">
+        <v>24.35</v>
+      </c>
+      <c r="H5" s="4">
+        <v>25.82</v>
+      </c>
+      <c r="I5" s="4">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="K5" s="4">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1096,20 +1166,34 @@
         <v>100003</v>
       </c>
       <c r="C6" s="4">
-        <v>4.18</v>
+        <v>843</v>
       </c>
       <c r="D6" s="4">
-        <v>57.5</v>
+        <v>19.7</v>
       </c>
       <c r="E6" s="4">
-        <v>0.377</v>
+        <v>61.88</v>
       </c>
       <c r="F6" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51.92</v>
+      </c>
+      <c r="G6" s="4">
+        <v>33.18</v>
+      </c>
+      <c r="H6" s="4">
+        <v>37.68</v>
+      </c>
+      <c r="I6" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="K6" s="4">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1117,20 +1201,34 @@
         <v>100004</v>
       </c>
       <c r="C7" s="4">
-        <v>1.49</v>
+        <v>451</v>
       </c>
       <c r="D7" s="4">
-        <v>21.2</v>
+        <v>9.1</v>
       </c>
       <c r="E7" s="4">
-        <v>0.44</v>
+        <v>70.34</v>
       </c>
       <c r="F7" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104.78</v>
+      </c>
+      <c r="G7" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="I7" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.248</v>
+      </c>
+      <c r="K7" s="4">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1138,20 +1236,34 @@
         <v>100005</v>
       </c>
       <c r="C8" s="4">
-        <v>4.6500000000000004</v>
+        <v>399.6</v>
       </c>
       <c r="D8" s="4">
-        <v>28.6</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4">
-        <v>0.48099999999999998</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="F8" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49.17</v>
+      </c>
+      <c r="G8" s="4">
+        <v>46.63</v>
+      </c>
+      <c r="H8" s="4">
+        <v>43.53</v>
+      </c>
+      <c r="I8" s="4">
+        <v>26.1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="K8" s="4">
+        <v>8.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1159,20 +1271,34 @@
         <v>100006</v>
       </c>
       <c r="C9" s="4">
-        <v>1.46</v>
+        <v>924</v>
       </c>
       <c r="D9" s="4">
-        <v>19.7</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4">
-        <v>0.6</v>
+        <v>66.02</v>
       </c>
       <c r="F9" s="4">
-        <v>0.21</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="G9" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>25.37</v>
+      </c>
+      <c r="I9" s="4">
+        <v>13.38</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="K9" s="4">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,20 +1306,34 @@
         <v>100007</v>
       </c>
       <c r="C10" s="4">
-        <v>5.9</v>
+        <v>284</v>
       </c>
       <c r="D10" s="4">
-        <v>38.799999999999997</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4">
-        <v>0.32900000000000001</v>
+        <v>63.85</v>
       </c>
       <c r="F10" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38.549999999999997</v>
+      </c>
+      <c r="G10" s="4">
+        <v>24.1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>26.04</v>
+      </c>
+      <c r="I10" s="4">
+        <v>26.85</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1201,20 +1341,34 @@
         <v>100008</v>
       </c>
       <c r="C11" s="4">
-        <v>1.63</v>
+        <v>443</v>
       </c>
       <c r="D11" s="4">
-        <v>23.9</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4">
-        <v>0.57999999999999996</v>
+        <v>66.45</v>
       </c>
       <c r="F11" s="4">
-        <v>0.27</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34.56</v>
+      </c>
+      <c r="G11" s="4">
+        <v>34.15</v>
+      </c>
+      <c r="H11" s="4">
+        <v>24.04</v>
+      </c>
+      <c r="I11" s="4">
+        <v>16</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K11" s="4">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1222,20 +1376,34 @@
         <v>100009</v>
       </c>
       <c r="C12" s="4">
-        <v>1.6</v>
+        <v>328</v>
       </c>
       <c r="D12" s="4">
-        <v>22.3</v>
+        <v>3</v>
       </c>
       <c r="E12" s="4">
-        <v>0.57899999999999996</v>
+        <v>74.06</v>
       </c>
       <c r="F12" s="4">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24.78</v>
+      </c>
+      <c r="G12" s="4">
+        <v>39.549999999999997</v>
+      </c>
+      <c r="H12" s="4">
+        <v>24.78</v>
+      </c>
+      <c r="I12" s="4">
+        <v>16.63</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="K12" s="4">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1243,18 +1411,32 @@
         <v>100010</v>
       </c>
       <c r="C13" s="4">
-        <v>4.71</v>
+        <v>709</v>
       </c>
       <c r="D13" s="4">
-        <v>47.7</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4">
-        <v>0.31900000000000001</v>
+        <v>64.48</v>
       </c>
       <c r="F13" s="4">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>47.18</v>
+      </c>
+      <c r="G13" s="4">
+        <v>33.159999999999997</v>
+      </c>
+      <c r="H13" s="4">
+        <v>28.71</v>
+      </c>
+      <c r="I13" s="4">
+        <v>19.98</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="4">
+        <v>9.36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>